<commit_message>
update Pablo 18 11
</commit_message>
<xml_diff>
--- a/AssignmentV2/Data/Generators_Existing.xlsx
+++ b/AssignmentV2/Data/Generators_Existing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxfavrot/Desktop/46750 Optimization in modern power systems/Assignment/Opti/AssignmentV2/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo Gutierrez\Desktop\Optimization in Modern Power Systems\Assignment\Opti\AssignmentV2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32CE158-4280-804E-AB2B-D3BA0FCCCE13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6A5ED1-C90B-49C2-90CC-DAFA620C87A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{6FC3F1B5-C6B9-44FB-8D40-D84BF8E2F66C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6FC3F1B5-C6B9-44FB-8D40-D84BF8E2F66C}"/>
   </bookViews>
   <sheets>
     <sheet name="Generators_AssetData_Existing" sheetId="2" r:id="rId1"/>
@@ -19,12 +19,25 @@
     <sheet name="Python_Gen_E_Data" sheetId="1" r:id="rId4"/>
     <sheet name="Python_Gen_E_Z_Data" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>P_max (MW)</t>
   </si>
@@ -121,12 +134,15 @@
   <si>
     <t>#Unit</t>
   </si>
+  <si>
+    <t>Capacity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -609,54 +625,53 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -990,13 +1005,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC2C505-C24B-4A6E-AD99-959D8FDC9DB0}">
   <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1012,7 +1027,7 @@
       <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
@@ -1067,7 +1082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1083,7 +1098,7 @@
       <c r="E2">
         <v>0.33</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>152</v>
       </c>
       <c r="G2">
@@ -1138,7 +1153,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1154,7 +1169,7 @@
       <c r="E3">
         <v>0.33</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
         <v>152</v>
       </c>
       <c r="G3">
@@ -1209,7 +1224,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1225,7 +1240,7 @@
       <c r="E4">
         <v>0.33</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
         <v>350</v>
       </c>
       <c r="G4">
@@ -1280,7 +1295,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1296,7 +1311,7 @@
       <c r="E5">
         <v>0.4</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5">
         <v>591</v>
       </c>
       <c r="G5">
@@ -1351,7 +1366,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1367,7 +1382,7 @@
       <c r="E6">
         <v>0.4</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6">
         <v>60</v>
       </c>
       <c r="G6">
@@ -1422,7 +1437,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1438,7 +1453,7 @@
       <c r="E7">
         <v>0.33</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7">
         <v>155</v>
       </c>
       <c r="G7">
@@ -1493,7 +1508,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1509,7 +1524,7 @@
       <c r="E8">
         <v>0.33</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8">
         <v>155</v>
       </c>
       <c r="G8">
@@ -1564,7 +1579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1580,7 +1595,7 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9">
         <v>400</v>
       </c>
       <c r="G9">
@@ -1635,7 +1650,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1651,7 +1666,7 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10">
         <v>400</v>
       </c>
       <c r="G10">
@@ -1706,7 +1721,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1722,7 +1737,7 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11">
         <v>300</v>
       </c>
       <c r="G11">
@@ -1777,7 +1792,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1793,7 +1808,7 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12">
         <v>310</v>
       </c>
       <c r="G12">
@@ -1848,7 +1863,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1864,7 +1879,7 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13">
         <v>350</v>
       </c>
       <c r="G13">
@@ -1919,7 +1934,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1935,7 +1950,7 @@
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14">
         <v>500</v>
       </c>
       <c r="G14">
@@ -1948,7 +1963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1964,7 +1979,7 @@
       <c r="E15">
         <v>0.4</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15">
         <v>100</v>
       </c>
       <c r="G15">
@@ -1977,7 +1992,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1993,7 +2008,7 @@
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16">
         <v>60</v>
       </c>
       <c r="G16">
@@ -2006,7 +2021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2022,7 +2037,7 @@
       <c r="E17">
         <v>0.35</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17">
         <v>200</v>
       </c>
       <c r="G17">
@@ -2035,10 +2050,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
-      <c r="F18" s="2"/>
-    </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -2091,7 +2103,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -2173,9 +2185,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2195,7 +2207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2215,7 +2227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2235,7 +2247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2255,7 +2267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2275,7 +2287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2295,7 +2307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2315,7 +2327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2335,7 +2347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2355,7 +2367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2375,7 +2387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2395,7 +2407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2415,7 +2427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2435,7 +2447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2455,7 +2467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2475,7 +2487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2495,7 +2507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2515,7 +2527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2535,7 +2547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2555,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2575,7 +2587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2595,7 +2607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2615,7 +2627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2635,7 +2647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2655,7 +2667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2675,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2695,7 +2707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2715,7 +2727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2735,7 +2747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2755,7 +2767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2775,7 +2787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2808,9 +2820,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -2818,7 +2830,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2826,7 +2838,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2834,15 +2846,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2850,7 +2862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2865,18 +2877,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79D5E8C-0F0A-428F-941D-8A7FA0E051FD}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -2886,8 +2899,11 @@
       <c r="C1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>Generators_AssetData_Existing!A2</f>
         <v>1</v>
@@ -2900,8 +2916,12 @@
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B2,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <f>Generators_AssetData_Existing!F2</f>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>Generators_AssetData_Existing!A3</f>
         <v>2</v>
@@ -2914,8 +2934,12 @@
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B3,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <f>Generators_AssetData_Existing!F3</f>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>Generators_AssetData_Existing!A4</f>
         <v>3</v>
@@ -2928,8 +2952,12 @@
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B4,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <f>Generators_AssetData_Existing!F4</f>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>Generators_AssetData_Existing!A5</f>
         <v>4</v>
@@ -2942,8 +2970,12 @@
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B5,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <f>Generators_AssetData_Existing!F5</f>
+        <v>591</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>Generators_AssetData_Existing!A6</f>
         <v>5</v>
@@ -2956,8 +2988,12 @@
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B6,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <f>Generators_AssetData_Existing!F6</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>Generators_AssetData_Existing!A7</f>
         <v>6</v>
@@ -2970,8 +3006,12 @@
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B7,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <f>Generators_AssetData_Existing!F7</f>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>Generators_AssetData_Existing!A8</f>
         <v>7</v>
@@ -2984,8 +3024,12 @@
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B8,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8">
+        <f>Generators_AssetData_Existing!F8</f>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>Generators_AssetData_Existing!A9</f>
         <v>8</v>
@@ -2998,8 +3042,12 @@
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B9,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9">
+        <f>Generators_AssetData_Existing!F9</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>Generators_AssetData_Existing!A10</f>
         <v>9</v>
@@ -3012,8 +3060,12 @@
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B10,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10">
+        <f>Generators_AssetData_Existing!F10</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>Generators_AssetData_Existing!A11</f>
         <v>10</v>
@@ -3026,8 +3078,12 @@
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B11,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11">
+        <f>Generators_AssetData_Existing!F11</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>Generators_AssetData_Existing!A12</f>
         <v>11</v>
@@ -3040,8 +3096,12 @@
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B12,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12">
+        <f>Generators_AssetData_Existing!F12</f>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>Generators_AssetData_Existing!A13</f>
         <v>12</v>
@@ -3054,8 +3114,12 @@
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B13,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13">
+        <f>Generators_AssetData_Existing!F13</f>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <f>Generators_AssetData_Existing!A14</f>
         <v>13</v>
@@ -3068,8 +3132,12 @@
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B14,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14">
+        <f>Generators_AssetData_Existing!F14</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <f>Generators_AssetData_Existing!A15</f>
         <v>14</v>
@@ -3082,8 +3150,12 @@
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B15,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15">
+        <f>Generators_AssetData_Existing!F15</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <f>Generators_AssetData_Existing!A16</f>
         <v>15</v>
@@ -3096,8 +3168,12 @@
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B16,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <f>Generators_AssetData_Existing!F16</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <f>Generators_AssetData_Existing!A17</f>
         <v>16</v>
@@ -3109,6 +3185,10 @@
       <c r="C17">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B17,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
         <v>40</v>
+      </c>
+      <c r="D17">
+        <f>Generators_AssetData_Existing!F17</f>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -3124,9 +3204,9 @@
       <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -3176,7 +3256,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>IF(Generators_AssetData_Existing!B$22=0,1,0)</f>
         <v>1</v>
@@ -3242,7 +3322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>IF(Generators_AssetData_Existing!B$22=1,1,0)</f>
         <v>0</v>

</xml_diff>

<commit_message>
Update Input Parameters LR v01
</commit_message>
<xml_diff>
--- a/AssignmentV2/Data/Generators_Existing.xlsx
+++ b/AssignmentV2/Data/Generators_Existing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo Gutierrez\Desktop\Optimization in Modern Power Systems\Assignment\Opti\AssignmentV2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonr\OneDrive\Documents\DTU\OptimizationInPS\ProjectGit\Opti\AssignmentV2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6A5ED1-C90B-49C2-90CC-DAFA620C87A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4856B977-7EE9-4DFB-8094-D7C9C16B77E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6FC3F1B5-C6B9-44FB-8D40-D84BF8E2F66C}"/>
+    <workbookView xWindow="40935" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="1" xr2:uid="{6FC3F1B5-C6B9-44FB-8D40-D84BF8E2F66C}"/>
   </bookViews>
   <sheets>
     <sheet name="Generators_AssetData_Existing" sheetId="2" r:id="rId1"/>
@@ -1006,12 +1006,12 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>0.33</v>
       </c>
       <c r="F2">
-        <v>152</v>
+        <v>1250</v>
       </c>
       <c r="G2">
         <v>30.4</v>
@@ -1153,7 +1153,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>0.33</v>
       </c>
       <c r="F3">
-        <v>152</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>30.4</v>
@@ -1224,7 +1224,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>0.33</v>
       </c>
       <c r="F4">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>75</v>
@@ -1295,7 +1295,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>0.4</v>
       </c>
       <c r="F5">
-        <v>591</v>
+        <v>1000</v>
       </c>
       <c r="G5">
         <v>206.85</v>
@@ -1366,7 +1366,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1374,58 +1374,58 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0.42899999999999999</v>
+        <v>0.98599999999999999</v>
       </c>
       <c r="E6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F6">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>12</v>
+        <v>54.25</v>
       </c>
       <c r="H6">
-        <v>40</v>
+        <v>155</v>
       </c>
       <c r="I6">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="J6">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="K6">
-        <v>60</v>
+        <v>155</v>
       </c>
       <c r="L6">
-        <v>60</v>
+        <v>155</v>
       </c>
       <c r="M6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N6">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O6">
-        <v>26.11</v>
+        <v>10.52</v>
       </c>
       <c r="P6">
+        <v>16</v>
+      </c>
+      <c r="Q6">
+        <v>14</v>
+      </c>
+      <c r="R6">
+        <v>16</v>
+      </c>
+      <c r="S6">
         <v>7</v>
       </c>
-      <c r="Q6">
-        <v>5</v>
-      </c>
-      <c r="R6">
-        <v>28</v>
-      </c>
-      <c r="S6">
-        <v>23</v>
-      </c>
       <c r="T6">
-        <v>437</v>
+        <v>312</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -1434,10 +1434,10 @@
         <v>0</v>
       </c>
       <c r="W6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1445,34 +1445,34 @@
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>0.98599999999999999</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>54.25</v>
+        <v>140</v>
       </c>
       <c r="H7">
-        <v>155</v>
+        <v>350</v>
       </c>
       <c r="I7">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="J7">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K7">
-        <v>155</v>
+        <v>240</v>
       </c>
       <c r="L7">
-        <v>155</v>
+        <v>240</v>
       </c>
       <c r="M7">
         <v>8</v>
@@ -1481,7 +1481,7 @@
         <v>8</v>
       </c>
       <c r="O7">
-        <v>10.52</v>
+        <v>10.89</v>
       </c>
       <c r="P7">
         <v>16</v>
@@ -1493,22 +1493,22 @@
         <v>16</v>
       </c>
       <c r="S7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T7">
-        <v>312</v>
+        <v>2298</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>280</v>
       </c>
       <c r="V7">
         <v>0</v>
       </c>
       <c r="W7">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1516,78 +1516,36 @@
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8">
-        <v>0.98599999999999999</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>54.25</v>
+        <v>50</v>
       </c>
       <c r="H8">
-        <v>155</v>
-      </c>
-      <c r="I8">
-        <v>30</v>
-      </c>
-      <c r="J8">
-        <v>30</v>
-      </c>
-      <c r="K8">
-        <v>155</v>
-      </c>
-      <c r="L8">
-        <v>155</v>
-      </c>
-      <c r="M8">
-        <v>8</v>
-      </c>
-      <c r="N8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O8">
-        <v>10.52</v>
-      </c>
-      <c r="P8">
-        <v>16</v>
-      </c>
-      <c r="Q8">
-        <v>14</v>
-      </c>
-      <c r="R8">
-        <v>16</v>
-      </c>
-      <c r="S8">
-        <v>7</v>
-      </c>
-      <c r="T8">
-        <v>312</v>
-      </c>
-      <c r="U8">
-        <v>124</v>
-      </c>
-      <c r="V8">
-        <v>1</v>
-      </c>
-      <c r="W8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1596,61 +1554,19 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="H9">
-        <v>200</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>280</v>
-      </c>
-      <c r="L9">
-        <v>280</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9">
-        <v>6.02</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>240</v>
-      </c>
-      <c r="V9">
-        <v>1</v>
-      </c>
-      <c r="W9">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1658,70 +1574,70 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F10">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="G10">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="H10">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K10">
-        <v>280</v>
+        <v>60</v>
       </c>
       <c r="L10">
-        <v>280</v>
+        <v>60</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O10">
-        <v>5.47</v>
+        <v>26.11</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>437</v>
       </c>
       <c r="U10">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="V10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1729,70 +1645,70 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>0.98599999999999999</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="F11">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="G11">
-        <v>300</v>
+        <v>54.25</v>
       </c>
       <c r="H11">
-        <v>300</v>
+        <v>155</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K11">
-        <v>300</v>
+        <v>155</v>
       </c>
       <c r="L11">
-        <v>300</v>
+        <v>155</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>10.52</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T11">
-        <v>0</v>
+        <v>312</v>
       </c>
       <c r="U11">
-        <v>240</v>
+        <v>124</v>
       </c>
       <c r="V11">
         <v>1</v>
       </c>
       <c r="W11">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1809,61 +1725,61 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>310</v>
+        <v>1500</v>
       </c>
       <c r="G12">
-        <v>108.5</v>
+        <v>100</v>
       </c>
       <c r="H12">
-        <v>310</v>
+        <v>200</v>
       </c>
       <c r="I12">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>180</v>
+        <v>280</v>
       </c>
       <c r="L12">
-        <v>180</v>
+        <v>280</v>
       </c>
       <c r="M12">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="N12">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="O12">
-        <v>10.52</v>
+        <v>6.02</v>
       </c>
       <c r="P12">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R12">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="S12">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="T12">
-        <v>624</v>
+        <v>0</v>
       </c>
       <c r="U12">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="V12">
         <v>1</v>
       </c>
       <c r="W12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1880,69 +1796,69 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="H13">
-        <v>350</v>
+        <v>200</v>
       </c>
       <c r="I13">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="K13">
+        <v>280</v>
+      </c>
+      <c r="L13">
+        <v>280</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>5.47</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
         <v>240</v>
       </c>
-      <c r="L13">
-        <v>240</v>
-      </c>
-      <c r="M13">
-        <v>8</v>
-      </c>
-      <c r="N13">
-        <v>8</v>
-      </c>
-      <c r="O13">
-        <v>10.89</v>
-      </c>
-      <c r="P13">
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13">
         <v>16</v>
       </c>
-      <c r="Q13">
-        <v>14</v>
-      </c>
-      <c r="R13">
-        <v>16</v>
-      </c>
-      <c r="S13">
-        <v>8</v>
-      </c>
-      <c r="T13">
-        <v>2298</v>
-      </c>
-      <c r="U13">
-        <v>280</v>
-      </c>
-      <c r="V13">
-        <v>0</v>
-      </c>
-      <c r="W13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1954,16 +1870,58 @@
         <v>500</v>
       </c>
       <c r="G14">
-        <v>50</v>
+        <v>300</v>
       </c>
       <c r="H14">
+        <v>300</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>300</v>
+      </c>
+      <c r="L14">
+        <v>300</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>240</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1971,57 +1929,96 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15">
-        <v>0.42899999999999999</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G15">
+        <v>108.5</v>
+      </c>
+      <c r="H15">
+        <v>310</v>
+      </c>
+      <c r="I15">
+        <v>60</v>
+      </c>
+      <c r="J15">
+        <v>60</v>
+      </c>
+      <c r="K15">
+        <v>180</v>
+      </c>
+      <c r="L15">
+        <v>180</v>
+      </c>
+      <c r="M15">
+        <v>8</v>
+      </c>
+      <c r="N15">
+        <v>8</v>
+      </c>
+      <c r="O15">
+        <v>10.52</v>
+      </c>
+      <c r="P15">
+        <v>17</v>
+      </c>
+      <c r="Q15">
+        <v>16</v>
+      </c>
+      <c r="R15">
+        <v>14</v>
+      </c>
+      <c r="S15">
+        <v>8</v>
+      </c>
+      <c r="T15">
+        <v>624</v>
+      </c>
+      <c r="U15">
+        <v>248</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15">
         <v>10</v>
       </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F16">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
-      <c r="O16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2038,7 +2035,7 @@
         <v>0.35</v>
       </c>
       <c r="F17">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <v>20</v>
@@ -2046,11 +2043,8 @@
       <c r="H17">
         <v>0</v>
       </c>
-      <c r="O17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -2103,7 +2097,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -2116,7 +2110,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="1">
-        <f>B4</f>
+        <f>B3</f>
         <v>0</v>
       </c>
       <c r="E22" s="1">
@@ -2137,7 +2131,7 @@
       </c>
       <c r="I22" s="1">
         <f>B9</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="1">
         <f>B10</f>
@@ -2157,7 +2151,7 @@
       </c>
       <c r="N22" s="1">
         <f>B14</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O22" s="1">
         <f>B15</f>
@@ -2165,7 +2159,7 @@
       </c>
       <c r="P22" s="1">
         <f>B16</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q22" s="1">
         <f>B17</f>
@@ -2181,13 +2175,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254540E5-F4F9-461A-915A-17335137E4D0}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2207,7 +2201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2227,7 +2221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2247,7 +2241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2267,7 +2261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2287,7 +2281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2307,7 +2301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2327,7 +2321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2347,7 +2341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2367,7 +2361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2387,7 +2381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2407,7 +2401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2427,7 +2421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2447,7 +2441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2467,7 +2461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2487,7 +2481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2507,7 +2501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2527,7 +2521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2547,7 +2541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2567,7 +2561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2587,7 +2581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2607,7 +2601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2627,7 +2621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2647,7 +2641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2667,7 +2661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2687,7 +2681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2707,7 +2701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2727,7 +2721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2747,7 +2741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2767,7 +2761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2787,7 +2781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2820,9 +2814,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -2830,23 +2824,23 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -2854,7 +2848,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2862,7 +2856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2879,17 +2873,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79D5E8C-0F0A-428F-941D-8A7FA0E051FD}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="2" max="2" width="12.19921875" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -2903,7 +2897,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <f>Generators_AssetData_Existing!A2</f>
         <v>1</v>
@@ -2914,14 +2908,14 @@
       </c>
       <c r="C2">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B2,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D2">
         <f>Generators_AssetData_Existing!F2</f>
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <f>Generators_AssetData_Existing!A3</f>
         <v>2</v>
@@ -2932,14 +2926,14 @@
       </c>
       <c r="C3">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B3,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D3">
         <f>Generators_AssetData_Existing!F3</f>
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <f>Generators_AssetData_Existing!A4</f>
         <v>3</v>
@@ -2950,14 +2944,14 @@
       </c>
       <c r="C4">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B4,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D4">
         <f>Generators_AssetData_Existing!F4</f>
-        <v>350</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5">
         <f>Generators_AssetData_Existing!A5</f>
         <v>4</v>
@@ -2968,75 +2962,75 @@
       </c>
       <c r="C5">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B5,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="D5">
         <f>Generators_AssetData_Existing!F5</f>
-        <v>591</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6">
         <f>Generators_AssetData_Existing!A6</f>
         <v>5</v>
       </c>
       <c r="B6" t="str">
         <f>Generators_AssetData_Existing!C6</f>
-        <v>Gas</v>
+        <v>Coal</v>
       </c>
       <c r="C6">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B6,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D6">
         <f>Generators_AssetData_Existing!F6</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7">
         <f>Generators_AssetData_Existing!A7</f>
         <v>6</v>
       </c>
       <c r="B7" t="str">
         <f>Generators_AssetData_Existing!C7</f>
-        <v>Coal</v>
+        <v>Wind</v>
       </c>
       <c r="C7">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B7,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <f>Generators_AssetData_Existing!F7</f>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8">
         <f>Generators_AssetData_Existing!A8</f>
         <v>7</v>
       </c>
       <c r="B8" t="str">
         <f>Generators_AssetData_Existing!C8</f>
-        <v>Coal</v>
+        <v>Wind</v>
       </c>
       <c r="C8">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B8,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <f>Generators_AssetData_Existing!F8</f>
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9">
         <f>Generators_AssetData_Existing!A9</f>
         <v>8</v>
       </c>
       <c r="B9" t="str">
         <f>Generators_AssetData_Existing!C9</f>
-        <v>Wind</v>
+        <v>PV</v>
       </c>
       <c r="C9">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B9,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
@@ -3044,46 +3038,46 @@
       </c>
       <c r="D9">
         <f>Generators_AssetData_Existing!F9</f>
-        <v>400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10">
         <f>Generators_AssetData_Existing!A10</f>
         <v>9</v>
       </c>
       <c r="B10" t="str">
         <f>Generators_AssetData_Existing!C10</f>
-        <v>Wind</v>
+        <v>Gas</v>
       </c>
       <c r="C10">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B10,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="D10">
         <f>Generators_AssetData_Existing!F10</f>
-        <v>400</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11">
         <f>Generators_AssetData_Existing!A11</f>
         <v>10</v>
       </c>
       <c r="B11" t="str">
         <f>Generators_AssetData_Existing!C11</f>
-        <v>PV</v>
+        <v>Coal</v>
       </c>
       <c r="C11">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B11,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="D11">
         <f>Generators_AssetData_Existing!F11</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12">
         <f>Generators_AssetData_Existing!A12</f>
         <v>11</v>
@@ -3098,10 +3092,10 @@
       </c>
       <c r="D12">
         <f>Generators_AssetData_Existing!F12</f>
-        <v>310</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13">
         <f>Generators_AssetData_Existing!A13</f>
         <v>12</v>
@@ -3116,17 +3110,17 @@
       </c>
       <c r="D13">
         <f>Generators_AssetData_Existing!F13</f>
-        <v>350</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14">
         <f>Generators_AssetData_Existing!A14</f>
         <v>13</v>
       </c>
       <c r="B14" t="str">
         <f>Generators_AssetData_Existing!C14</f>
-        <v>Wind</v>
+        <v>PV</v>
       </c>
       <c r="C14">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B14,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
@@ -3137,43 +3131,43 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15">
         <f>Generators_AssetData_Existing!A15</f>
         <v>14</v>
       </c>
       <c r="B15" t="str">
         <f>Generators_AssetData_Existing!C15</f>
-        <v>Gas</v>
+        <v>Wind</v>
       </c>
       <c r="C15">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B15,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <f>Generators_AssetData_Existing!F15</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16">
         <f>Generators_AssetData_Existing!A16</f>
         <v>15</v>
       </c>
       <c r="B16" t="str">
         <f>Generators_AssetData_Existing!C16</f>
-        <v>PV</v>
+        <v>Gas</v>
       </c>
       <c r="C16">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B16,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="D16">
         <f>Generators_AssetData_Existing!F16</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17">
         <f>Generators_AssetData_Existing!A17</f>
         <v>16</v>
@@ -3184,11 +3178,11 @@
       </c>
       <c r="C17">
         <f>INDEX(Fuel_Cost_Absolute!$B$2:$B$6,MATCH( Python_Gen_E_Data!B17,Fuel_Cost_Absolute!$A$2:$A$6,0))</f>
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D17">
         <f>Generators_AssetData_Existing!F17</f>
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3201,12 +3195,12 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>1</v>
       </c>
@@ -3256,7 +3250,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2">
         <f>IF(Generators_AssetData_Existing!B$22=0,1,0)</f>
         <v>1</v>
@@ -3287,7 +3281,7 @@
       </c>
       <c r="H2">
         <f>IF(Generators_AssetData_Existing!I$22=0,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <f>IF(Generators_AssetData_Existing!J$22=0,1,0)</f>
@@ -3307,7 +3301,7 @@
       </c>
       <c r="M2">
         <f>IF(Generators_AssetData_Existing!N$22=0,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2">
         <f>IF(Generators_AssetData_Existing!O$22=0,1,0)</f>
@@ -3315,14 +3309,14 @@
       </c>
       <c r="O2">
         <f>IF(Generators_AssetData_Existing!P$22=0,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <f>IF(Generators_AssetData_Existing!Q$22=0,1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3">
         <f>IF(Generators_AssetData_Existing!B$22=1,1,0)</f>
         <v>0</v>
@@ -3353,7 +3347,7 @@
       </c>
       <c r="H3">
         <f>IF(Generators_AssetData_Existing!I$22=1,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <f>IF(Generators_AssetData_Existing!J$22=1,1,0)</f>
@@ -3373,7 +3367,7 @@
       </c>
       <c r="M3">
         <f>IF(Generators_AssetData_Existing!N$22=1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
         <f>IF(Generators_AssetData_Existing!O$22=1,1,0)</f>
@@ -3381,7 +3375,7 @@
       </c>
       <c r="O3">
         <f>IF(Generators_AssetData_Existing!P$22=1,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3">
         <f>IF(Generators_AssetData_Existing!Q$22=1,1,0)</f>

</xml_diff>

<commit_message>
Înput Data Base Case
</commit_message>
<xml_diff>
--- a/AssignmentV2/Data/Generators_Existing.xlsx
+++ b/AssignmentV2/Data/Generators_Existing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonr\OneDrive\Documents\DTU\OptimizationInPS\ProjectGit\Opti\AssignmentV2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4856B977-7EE9-4DFB-8094-D7C9C16B77E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E983D83F-2291-4877-8A76-8A4C60C2D4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40935" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="1" xr2:uid="{6FC3F1B5-C6B9-44FB-8D40-D84BF8E2F66C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{6FC3F1B5-C6B9-44FB-8D40-D84BF8E2F66C}"/>
   </bookViews>
   <sheets>
     <sheet name="Generators_AssetData_Existing" sheetId="2" r:id="rId1"/>
@@ -1005,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC2C505-C24B-4A6E-AD99-959D8FDC9DB0}">
   <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2175,8 +2175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254540E5-F4F9-461A-915A-17335137E4D0}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>